<commit_message>
additional updates to calculate statistics, more control variables, more in-line comments
</commit_message>
<xml_diff>
--- a/data/marijuana applicants test data - correct matches.xlsx
+++ b/data/marijuana applicants test data - correct matches.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$630</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$629</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="6">
   <si>
     <t>Exact</t>
   </si>
@@ -362,11 +362,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C630"/>
+  <dimension ref="A1:C629"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A593" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A630" sqref="A630"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7197,10 +7197,10 @@
     </row>
     <row r="621" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A621">
-        <v>734</v>
+        <v>735</v>
       </c>
       <c r="B621">
-        <v>655</v>
+        <v>657</v>
       </c>
       <c r="C621" t="s">
         <v>0</v>
@@ -7208,10 +7208,10 @@
     </row>
     <row r="622" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A622">
-        <v>735</v>
+        <v>736</v>
       </c>
       <c r="B622">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="C622" t="s">
         <v>0</v>
@@ -7219,10 +7219,10 @@
     </row>
     <row r="623" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A623">
-        <v>736</v>
+        <v>737</v>
       </c>
       <c r="B623">
-        <v>658</v>
+        <v>659</v>
       </c>
       <c r="C623" t="s">
         <v>0</v>
@@ -7230,10 +7230,10 @@
     </row>
     <row r="624" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A624">
-        <v>737</v>
+        <v>738</v>
       </c>
       <c r="B624">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="C624" t="s">
         <v>0</v>
@@ -7241,10 +7241,10 @@
     </row>
     <row r="625" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A625">
-        <v>738</v>
+        <v>740</v>
       </c>
       <c r="B625">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="C625" t="s">
         <v>0</v>
@@ -7252,10 +7252,10 @@
     </row>
     <row r="626" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A626">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="B626">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="C626" t="s">
         <v>0</v>
@@ -7263,10 +7263,10 @@
     </row>
     <row r="627" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A627">
-        <v>741</v>
+        <v>743</v>
       </c>
       <c r="B627">
-        <v>662</v>
+        <v>663</v>
       </c>
       <c r="C627" t="s">
         <v>0</v>
@@ -7274,10 +7274,10 @@
     </row>
     <row r="628" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A628">
-        <v>743</v>
+        <v>744</v>
       </c>
       <c r="B628">
-        <v>663</v>
+        <v>664</v>
       </c>
       <c r="C628" t="s">
         <v>0</v>
@@ -7285,28 +7285,17 @@
     </row>
     <row r="629" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A629">
-        <v>744</v>
+        <v>160</v>
       </c>
       <c r="B629">
-        <v>664</v>
+        <v>147</v>
       </c>
       <c r="C629" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="630" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A630">
-        <v>160</v>
-      </c>
-      <c r="B630">
-        <v>147</v>
-      </c>
-      <c r="C630" t="s">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C630"/>
+  <autoFilter ref="A1:C629"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
re-ran master_file with new tagged marijuana applicants test data
</commit_message>
<xml_diff>
--- a/data/marijuana applicants test data - correct matches.xlsx
+++ b/data/marijuana applicants test data - correct matches.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alan\Documents\GitHub\CS410-Project\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11535" windowHeight="10260"/>
   </bookViews>
@@ -15,9 +10,9 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$629</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$628</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="630" uniqueCount="6">
   <si>
     <t>Exact</t>
   </si>
@@ -354,7 +349,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -362,11 +357,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C629"/>
+  <dimension ref="A1:C628"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <pane ySplit="1" topLeftCell="A592" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A629" sqref="A629"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1953,7 +1948,7 @@
         <v>160</v>
       </c>
       <c r="B144">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="C144" t="s">
         <v>0</v>
@@ -7283,19 +7278,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="629" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A629">
-        <v>160</v>
-      </c>
-      <c r="B629">
-        <v>147</v>
-      </c>
-      <c r="C629" t="s">
-        <v>1</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:C629"/>
+  <autoFilter ref="A1:C628"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
slight change to aggregate functions to include zip5 Exact as a value for the groundtruth matches.  Slight changes to the doc strings in various files.  Re-ran master_file to ensure no bugs.  updates to documentation in readme.md and address_compare.rst
</commit_message>
<xml_diff>
--- a/data/marijuana applicants test data - correct matches.xlsx
+++ b/data/marijuana applicants test data - correct matches.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alan\Documents\GitHub\CS410-Project\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11535" windowHeight="10260"/>
   </bookViews>
@@ -22,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="630" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="633" uniqueCount="7">
   <si>
     <t>Exact</t>
   </si>
@@ -40,6 +45,9 @@
   </si>
   <si>
     <t>Record_ID_list_2</t>
+  </si>
+  <si>
+    <t>Zip5 Exact</t>
   </si>
 </sst>
 </file>
@@ -349,7 +357,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -357,11 +365,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C628"/>
+  <dimension ref="A1:C631"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A592" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A629" sqref="A629"/>
+      <pane ySplit="1" topLeftCell="A621" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C630" sqref="C630:C631"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7278,6 +7286,39 @@
         <v>0</v>
       </c>
     </row>
+    <row r="629" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A629">
+        <v>196</v>
+      </c>
+      <c r="B629">
+        <v>666</v>
+      </c>
+      <c r="C629" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="630" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A630">
+        <v>306</v>
+      </c>
+      <c r="B630">
+        <v>555</v>
+      </c>
+      <c r="C630" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="631" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A631">
+        <v>616</v>
+      </c>
+      <c r="B631">
+        <v>284</v>
+      </c>
+      <c r="C631" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:C628"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>